<commit_message>
Change last transaction checkpoint
</commit_message>
<xml_diff>
--- a/FinX_billPayment/Default.xlsx
+++ b/FinX_billPayment/Default.xlsx
@@ -17,18 +17,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
-    <t>payment</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
     <t>fromAccount</t>
   </si>
   <si>
     <t>5fbe3b2c4b2ce7c51a3d775df35f</t>
   </si>
   <si>
+    <t>water</t>
+  </si>
+  <si>
     <t>userName</t>
   </si>
   <si>
@@ -45,6 +42,9 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Test Payment</t>
   </si>
   <si>
     <t>543875</t>
@@ -245,10 +245,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
@@ -554,7 +554,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -562,7 +562,7 @@
     <col min="1" max="1" width="27.56640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.98828125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.1015625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.8671875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.41796875" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9.078125" style="2" customWidth="1"/>
@@ -570,42 +570,42 @@
   <sheetData>
     <row customFormat="1">
       <c t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c t="s">
+        <v>7</v>
       </c>
       <c t="s">
         <v>8</v>
       </c>
       <c t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c t="s">
+        <v>0</v>
       </c>
       <c t="s">
         <v>5</v>
-      </c>
-      <c t="s">
-        <v>2</v>
-      </c>
-      <c t="s">
-        <v>6</v>
       </c>
     </row>
     <row>
       <c s="1" t="s">
-        <v>3</v>
-      </c>
-      <c s="4" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c s="3" t="s">
+        <v>6</v>
       </c>
       <c s="1">
         <v>5</v>
       </c>
       <c s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c s="5" t="s">
         <v>10</v>
       </c>
-      <c s="3" t="s">
-        <v>1</v>
+      <c s="4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>